<commit_message>
Update Excel documentation file.
</commit_message>
<xml_diff>
--- a/datasets.xlsx
+++ b/datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StuehlerH/zeppelin/PhD/07_Implementierungen/02_ZPAI/pre-postprocessing-evaluation-framework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B199197-3F14-874F-8096-6722D7B6EF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59E7B6A-E1C2-2444-BC77-B81724B676AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51220" yWindow="-7500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{44082038-FCD4-C940-8E68-2A17959B9171}"/>
+    <workbookView xWindow="-51200" yWindow="-7500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{44082038-FCD4-C940-8E68-2A17959B9171}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Measurement data</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>Use a boxplot to depict automl MAPE values.</t>
+  </si>
+  <si>
+    <t>merged-files-final-selected-features-2023-12-12</t>
+  </si>
+  <si>
+    <t>Automatic IQR OD</t>
+  </si>
+  <si>
+    <t>merged-files-final-2023-12-12</t>
+  </si>
+  <si>
+    <t>Calculated on Linux Home</t>
+  </si>
+  <si>
+    <t>Calculated on Linux ZZ</t>
   </si>
 </sst>
 </file>
@@ -112,7 +127,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,6 +156,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -162,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -186,9 +209,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC4C17-4148-484F-AB65-A037E96590BF}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,6 +651,34 @@
         <v>15</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="10">
+        <v>2804</v>
+      </c>
+      <c r="C9" s="10">
+        <v>17</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="10">
+        <v>2804</v>
+      </c>
+      <c r="C10" s="10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -639,10 +689,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B5D745-8D7E-5345-8D46-5816273A76D4}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,7 +735,7 @@
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -724,8 +774,36 @@
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>45272</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>45273</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>